<commit_message>
Added dynamic loading calcs
Table 5 and 6 seem to work, but not sure about sign convention
</commit_message>
<xml_diff>
--- a/designer/i1s45285545.xlsx
+++ b/designer/i1s45285545.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teode\GitHub\mech2100-a2\designer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B232C0F-69F9-42E7-82AA-73E185332DD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD9979D-07F9-4DF2-ADDC-4814C2F59CFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4200" yWindow="-11115" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1671,9 +1671,15 @@
       <c r="E66" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
+      <c r="F66" s="11">
+        <v>49513.722756633695</v>
+      </c>
+      <c r="G66" s="11">
+        <v>66587.420258921178</v>
+      </c>
+      <c r="H66" s="11">
+        <v>201469.63052699226</v>
+      </c>
       <c r="J66" s="2" t="s">
         <v>95</v>
       </c>
@@ -1691,9 +1697,15 @@
       <c r="E67" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
+      <c r="F67" s="11">
+        <v>29708.23365398022</v>
+      </c>
+      <c r="G67" s="11">
+        <v>39952.452155352716</v>
+      </c>
+      <c r="H67" s="11">
+        <v>120881.77831619537</v>
+      </c>
       <c r="J67" s="2" t="s">
         <v>95</v>
       </c>
@@ -1711,9 +1723,15 @@
       <c r="E68" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
+      <c r="F68" s="11">
+        <v>9902.7445513267448</v>
+      </c>
+      <c r="G68" s="11">
+        <v>13317.484051784249</v>
+      </c>
+      <c r="H68" s="11">
+        <v>40293.926105398481</v>
+      </c>
       <c r="J68" s="2" t="s">
         <v>95</v>
       </c>
@@ -1731,9 +1749,15 @@
       <c r="E69" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
+      <c r="F69" s="11">
+        <v>-39610.978205306958</v>
+      </c>
+      <c r="G69" s="11">
+        <v>-53269.936207136947</v>
+      </c>
+      <c r="H69" s="11">
+        <v>-161175.70442159381</v>
+      </c>
       <c r="J69" s="2" t="s">
         <v>95</v>
       </c>
@@ -1751,9 +1775,15 @@
       <c r="E70" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
+      <c r="F70" s="11">
+        <v>-19805.489102653482</v>
+      </c>
+      <c r="G70" s="11">
+        <v>-26634.968103568481</v>
+      </c>
+      <c r="H70" s="11">
+        <v>-80587.852210796918</v>
+      </c>
       <c r="J70" s="2" t="s">
         <v>95</v>
       </c>
@@ -1771,9 +1801,15 @@
       <c r="E71" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
+      <c r="F71" s="11">
+        <v>0</v>
+      </c>
+      <c r="G71" s="11">
+        <v>0</v>
+      </c>
+      <c r="H71" s="11">
+        <v>0</v>
+      </c>
       <c r="J71" s="2" t="s">
         <v>95</v>
       </c>
@@ -1791,9 +1827,15 @@
       <c r="E72" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
+      <c r="F72" s="11">
+        <v>16504.57425221123</v>
+      </c>
+      <c r="G72" s="11">
+        <v>22195.806752973727</v>
+      </c>
+      <c r="H72" s="11">
+        <v>67156.54350899742</v>
+      </c>
       <c r="J72" s="2" t="s">
         <v>95</v>
       </c>
@@ -1811,9 +1853,15 @@
       <c r="E73" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
+      <c r="F73" s="11">
+        <v>-19247.475701909207</v>
+      </c>
+      <c r="G73" s="11">
+        <v>-25884.536288774452</v>
+      </c>
+      <c r="H73" s="11">
+        <v>-78317.314925009865</v>
+      </c>
       <c r="J73" s="2" t="s">
         <v>95</v>
       </c>
@@ -1831,9 +1879,15 @@
       <c r="E74" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
+      <c r="F74" s="11">
+        <v>19247.475701909207</v>
+      </c>
+      <c r="G74" s="11">
+        <v>25884.536288774452</v>
+      </c>
+      <c r="H74" s="11">
+        <v>78317.314925009865</v>
+      </c>
       <c r="J74" s="2" t="s">
         <v>95</v>
       </c>
@@ -1851,9 +1905,15 @@
       <c r="E75" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
+      <c r="F75" s="11">
+        <v>-19247.475701909207</v>
+      </c>
+      <c r="G75" s="11">
+        <v>-25884.536288774452</v>
+      </c>
+      <c r="H75" s="11">
+        <v>-78317.314925009865</v>
+      </c>
       <c r="J75" s="2" t="s">
         <v>95</v>
       </c>
@@ -1871,9 +1931,15 @@
       <c r="E76" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
+      <c r="F76" s="11">
+        <v>19247.475701909207</v>
+      </c>
+      <c r="G76" s="11">
+        <v>25884.536288774452</v>
+      </c>
+      <c r="H76" s="11">
+        <v>78317.314925009865</v>
+      </c>
       <c r="J76" s="2" t="s">
         <v>95</v>
       </c>
@@ -1891,9 +1957,15 @@
       <c r="E77" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
+      <c r="F77" s="11">
+        <v>-19247.475701909207</v>
+      </c>
+      <c r="G77" s="11">
+        <v>-25884.536288774452</v>
+      </c>
+      <c r="H77" s="11">
+        <v>-78317.314925009865</v>
+      </c>
       <c r="J77" s="2" t="s">
         <v>95</v>
       </c>
@@ -1911,9 +1983,15 @@
       <c r="E78" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
+      <c r="F78" s="11">
+        <v>16504.57425221123</v>
+      </c>
+      <c r="G78" s="11">
+        <v>22195.806752973727</v>
+      </c>
+      <c r="H78" s="11">
+        <v>67156.54350899742</v>
+      </c>
       <c r="J78" s="2" t="s">
         <v>95</v>
       </c>
@@ -1990,9 +2068,15 @@
       <c r="E85" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
+      <c r="F85" s="11">
+        <v>-49513.722756633695</v>
+      </c>
+      <c r="G85" s="11">
+        <v>-66587.420258921178</v>
+      </c>
+      <c r="H85" s="11">
+        <v>-201469.63052699226</v>
+      </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
@@ -2007,9 +2091,15 @@
       <c r="E86" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
+      <c r="F86" s="11">
+        <v>16504.57425221123</v>
+      </c>
+      <c r="G86" s="11">
+        <v>22195.806752973727</v>
+      </c>
+      <c r="H86" s="11">
+        <v>67156.54350899742</v>
+      </c>
       <c r="J86" s="2" t="s">
         <v>87</v>
       </c>
@@ -2027,9 +2117,15 @@
       <c r="E87" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
+      <c r="F87" s="11">
+        <v>49513.722756633695</v>
+      </c>
+      <c r="G87" s="11">
+        <v>66587.420258921178</v>
+      </c>
+      <c r="H87" s="11">
+        <v>201469.63052699226</v>
+      </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
@@ -2044,9 +2140,15 @@
       <c r="E88" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
+      <c r="F88" s="11">
+        <v>0</v>
+      </c>
+      <c r="G88" s="11">
+        <v>0</v>
+      </c>
+      <c r="H88" s="11">
+        <v>0</v>
+      </c>
       <c r="J88" s="2" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Added physical results calcs
Signs have been changed, things still in contention
</commit_message>
<xml_diff>
--- a/designer/i1s45285545.xlsx
+++ b/designer/i1s45285545.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teode\GitHub\mech2100-a2\designer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD9979D-07F9-4DF2-ADDC-4814C2F59CFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F01AC0-61FF-4FDE-911C-8CB2FCEEAE90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="L92" sqref="L92"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="H136" sqref="H136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1259,13 +1259,13 @@
         <v>49</v>
       </c>
       <c r="F25" s="11">
-        <v>-33009.148504422461</v>
+        <v>33009.148504422461</v>
       </c>
       <c r="G25" s="11">
-        <v>-44391.613505947455</v>
+        <v>44391.613505947455</v>
       </c>
       <c r="H25" s="11">
-        <v>-134313.08701799484</v>
+        <v>134313.08701799484</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="2" t="s">
@@ -1672,13 +1672,13 @@
         <v>94</v>
       </c>
       <c r="F66" s="11">
-        <v>49513.722756633695</v>
+        <v>-49513.722756633695</v>
       </c>
       <c r="G66" s="11">
-        <v>66587.420258921178</v>
+        <v>-66587.420258921178</v>
       </c>
       <c r="H66" s="11">
-        <v>201469.63052699226</v>
+        <v>-201469.63052699226</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>95</v>
@@ -1698,13 +1698,13 @@
         <v>94</v>
       </c>
       <c r="F67" s="11">
-        <v>29708.23365398022</v>
+        <v>-29708.23365398022</v>
       </c>
       <c r="G67" s="11">
-        <v>39952.452155352716</v>
+        <v>-39952.452155352716</v>
       </c>
       <c r="H67" s="11">
-        <v>120881.77831619537</v>
+        <v>-120881.77831619537</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>95</v>
@@ -1724,13 +1724,13 @@
         <v>94</v>
       </c>
       <c r="F68" s="11">
-        <v>9902.7445513267448</v>
+        <v>-9902.7445513267448</v>
       </c>
       <c r="G68" s="11">
-        <v>13317.484051784249</v>
+        <v>-13317.484051784249</v>
       </c>
       <c r="H68" s="11">
-        <v>40293.926105398481</v>
+        <v>-40293.926105398481</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>95</v>
@@ -1750,13 +1750,13 @@
         <v>94</v>
       </c>
       <c r="F69" s="11">
-        <v>-39610.978205306958</v>
+        <v>39610.978205306958</v>
       </c>
       <c r="G69" s="11">
-        <v>-53269.936207136947</v>
+        <v>53269.936207136947</v>
       </c>
       <c r="H69" s="11">
-        <v>-161175.70442159381</v>
+        <v>161175.70442159381</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>95</v>
@@ -1776,13 +1776,13 @@
         <v>94</v>
       </c>
       <c r="F70" s="11">
-        <v>-19805.489102653482</v>
+        <v>19805.489102653482</v>
       </c>
       <c r="G70" s="11">
-        <v>-26634.968103568481</v>
+        <v>26634.968103568481</v>
       </c>
       <c r="H70" s="11">
-        <v>-80587.852210796918</v>
+        <v>80587.852210796918</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>95</v>
@@ -1828,13 +1828,13 @@
         <v>94</v>
       </c>
       <c r="F72" s="11">
-        <v>16504.57425221123</v>
+        <v>-16504.57425221123</v>
       </c>
       <c r="G72" s="11">
-        <v>22195.806752973727</v>
+        <v>-22195.806752973727</v>
       </c>
       <c r="H72" s="11">
-        <v>67156.54350899742</v>
+        <v>-67156.54350899742</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>95</v>
@@ -1854,13 +1854,13 @@
         <v>94</v>
       </c>
       <c r="F73" s="11">
-        <v>-19247.475701909207</v>
+        <v>19247.475701909207</v>
       </c>
       <c r="G73" s="11">
-        <v>-25884.536288774452</v>
+        <v>25884.536288774452</v>
       </c>
       <c r="H73" s="11">
-        <v>-78317.314925009865</v>
+        <v>78317.314925009865</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>95</v>
@@ -1880,13 +1880,13 @@
         <v>94</v>
       </c>
       <c r="F74" s="11">
-        <v>19247.475701909207</v>
+        <v>-19247.475701909207</v>
       </c>
       <c r="G74" s="11">
-        <v>25884.536288774452</v>
+        <v>-25884.536288774452</v>
       </c>
       <c r="H74" s="11">
-        <v>78317.314925009865</v>
+        <v>-78317.314925009865</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>95</v>
@@ -1906,13 +1906,13 @@
         <v>94</v>
       </c>
       <c r="F75" s="11">
-        <v>-19247.475701909207</v>
+        <v>19247.475701909207</v>
       </c>
       <c r="G75" s="11">
-        <v>-25884.536288774452</v>
+        <v>25884.536288774452</v>
       </c>
       <c r="H75" s="11">
-        <v>-78317.314925009865</v>
+        <v>78317.314925009865</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>95</v>
@@ -1932,13 +1932,13 @@
         <v>94</v>
       </c>
       <c r="F76" s="11">
-        <v>19247.475701909207</v>
+        <v>-19247.475701909207</v>
       </c>
       <c r="G76" s="11">
-        <v>25884.536288774452</v>
+        <v>-25884.536288774452</v>
       </c>
       <c r="H76" s="11">
-        <v>78317.314925009865</v>
+        <v>-78317.314925009865</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>95</v>
@@ -1958,13 +1958,13 @@
         <v>94</v>
       </c>
       <c r="F77" s="11">
-        <v>-19247.475701909207</v>
+        <v>19247.475701909207</v>
       </c>
       <c r="G77" s="11">
-        <v>-25884.536288774452</v>
+        <v>25884.536288774452</v>
       </c>
       <c r="H77" s="11">
-        <v>-78317.314925009865</v>
+        <v>78317.314925009865</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>95</v>
@@ -1984,13 +1984,13 @@
         <v>94</v>
       </c>
       <c r="F78" s="11">
-        <v>16504.57425221123</v>
+        <v>-16504.57425221123</v>
       </c>
       <c r="G78" s="11">
-        <v>22195.806752973727</v>
+        <v>-22195.806752973727</v>
       </c>
       <c r="H78" s="11">
-        <v>67156.54350899742</v>
+        <v>-67156.54350899742</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>95</v>
@@ -2225,9 +2225,15 @@
       <c r="E101" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
+      <c r="F101" s="11">
+        <v>17.385849761672155</v>
+      </c>
+      <c r="G101" s="11">
+        <v>23.380970369145317</v>
+      </c>
+      <c r="H101" s="11">
+        <v>70.742423168183237</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
@@ -2242,9 +2248,15 @@
       <c r="E102" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
+      <c r="F102" s="11">
+        <v>-30.014999999999997</v>
+      </c>
+      <c r="G102" s="11">
+        <v>-40.365000000000002</v>
+      </c>
+      <c r="H102" s="11">
+        <v>-122.12999999999997</v>
+      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
@@ -2259,9 +2271,15 @@
       <c r="E103" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
+      <c r="F103" s="11">
+        <v>8.6929248808360793</v>
+      </c>
+      <c r="G103" s="11">
+        <v>11.69048518457266</v>
+      </c>
+      <c r="H103" s="11">
+        <v>35.371211584091625</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
@@ -2276,9 +2294,15 @@
       <c r="E104" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
+      <c r="F104" s="11">
+        <v>30.014999999999997</v>
+      </c>
+      <c r="G104" s="11">
+        <v>40.365000000000002</v>
+      </c>
+      <c r="H104" s="11">
+        <v>122.12999999999997</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C109" s="2" t="s">
@@ -2301,7 +2325,9 @@
       <c r="E110" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F110" s="11"/>
+      <c r="F110" s="11">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
@@ -2313,7 +2339,9 @@
       <c r="E111" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F111" s="11"/>
+      <c r="F111" s="11">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
@@ -2325,7 +2353,9 @@
       <c r="E112" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F112" s="11"/>
+      <c r="F112" s="11">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
@@ -2337,7 +2367,9 @@
       <c r="E113" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F113" s="11"/>
+      <c r="F113" s="11">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C120" s="2" t="s">
@@ -2411,9 +2443,15 @@
       <c r="E125" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
+      <c r="F125" s="11">
+        <v>26.078774642508233</v>
+      </c>
+      <c r="G125" s="11">
+        <v>35.071455553717968</v>
+      </c>
+      <c r="H125" s="11">
+        <v>106.11363475227486</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
@@ -2428,9 +2466,15 @@
       <c r="E126" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F126" s="11"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="11"/>
+      <c r="F126" s="11">
+        <v>-36.017999999999994</v>
+      </c>
+      <c r="G126" s="11">
+        <v>-48.438000000000002</v>
+      </c>
+      <c r="H126" s="11">
+        <v>-146.55599999999998</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
@@ -2445,9 +2489,15 @@
       <c r="E127" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F127" s="11"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
+      <c r="F127" s="11">
+        <v>13.03938732125412</v>
+      </c>
+      <c r="G127" s="11">
+        <v>17.535727776858987</v>
+      </c>
+      <c r="H127" s="11">
+        <v>53.056817376137438</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
@@ -2462,9 +2512,15 @@
       <c r="E128" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F128" s="11"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="11"/>
+      <c r="F128" s="11">
+        <v>36.017999999999994</v>
+      </c>
+      <c r="G128" s="11">
+        <v>48.438000000000002</v>
+      </c>
+      <c r="H128" s="11">
+        <v>146.55599999999998</v>
+      </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C134" s="2" t="s">
@@ -2490,7 +2546,9 @@
       <c r="E135" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F135" s="11"/>
+      <c r="F135" s="11">
+        <v>3258.721877189379</v>
+      </c>
       <c r="H135" s="2" t="s">
         <v>127</v>
       </c>
@@ -2508,7 +2566,9 @@
       <c r="E136" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F136" s="11"/>
+      <c r="F136" s="11">
+        <v>33.582666144355763</v>
+      </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
@@ -2523,7 +2583,9 @@
       <c r="E137" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F137" s="11"/>
+      <c r="F137" s="11">
+        <v>32.750118334874607</v>
+      </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>

</xml_diff>

<commit_message>
Standardised the sign convention
</commit_message>
<xml_diff>
--- a/designer/i1s45285545.xlsx
+++ b/designer/i1s45285545.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teode\GitHub\mech2100-a2\designer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F01AC0-61FF-4FDE-911C-8CB2FCEEAE90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF3839E-B61B-413A-9E23-3BC3C6CCDC21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6180" yWindow="-19560" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changed stress calcs to range
Changed nominal stress calculation from  peak stress to stress range.
</commit_message>
<xml_diff>
--- a/designer/i1s45285545.xlsx
+++ b/designer/i1s45285545.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teode\GitHub\mech2100-a2\designer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF3839E-B61B-413A-9E23-3BC3C6CCDC21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8240573-0AAC-4657-958C-C45E113C7A04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6180" yWindow="-19560" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="M131" sqref="M131"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2249,13 +2249,13 @@
         <v>117</v>
       </c>
       <c r="F102" s="11">
-        <v>-30.014999999999997</v>
+        <v>30.014999999999997</v>
       </c>
       <c r="G102" s="11">
-        <v>-40.365000000000002</v>
+        <v>40.365000000000002</v>
       </c>
       <c r="H102" s="11">
-        <v>-122.12999999999997</v>
+        <v>122.12999999999997</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -2467,13 +2467,13 @@
         <v>122</v>
       </c>
       <c r="F126" s="11">
-        <v>-36.017999999999994</v>
+        <v>36.017999999999994</v>
       </c>
       <c r="G126" s="11">
-        <v>-48.438000000000002</v>
+        <v>48.438000000000002</v>
       </c>
       <c r="H126" s="11">
-        <v>-146.55599999999998</v>
+        <v>146.55599999999998</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added note on pin calculation
</commit_message>
<xml_diff>
--- a/designer/i1s45285545.xlsx
+++ b/designer/i1s45285545.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teode\GitHub\mech2100-a2\designer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8240573-0AAC-4657-958C-C45E113C7A04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C82F16-F395-4BF8-BA0E-5A3BB9079B63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>

</xml_diff>